<commit_message>
update ig and CapabilityStatement
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/data-source-client.xlsx
+++ b/input/resources-spreadsheet/data-source-client.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/Davinci-CDEX/input/resources-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D50DBC5-AF31-0E4F-BF1E-79D52569504C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B81858-F0EF-CB46-9C2E-8AC119301BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="460" windowWidth="26840" windowHeight="17540" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="460" windowWidth="26840" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -462,11 +462,6 @@
 1. For security considerations specific to this guide refer to the [Security and Privacy](security.html) section.</t>
   </si>
   <si>
-    <t>1. POSTing the `$submit-attachment` operation to exchange clinical data using a FHIR based Attachments transaction.
-1. Query for Authorization information represented by a CommunicationRequest or ServiceRequest.
-1. Posting a subscription notification to a Data Consumer endpoint updating the status of a Task.</t>
-  </si>
-  <si>
     <t>The  Da Vinci CDex Data Source **SHALL**:
 1. Support at least one of the these FHIR transaction approaches for exchanging clinical information as defined in this Guide:
      1. Task Based Approach
@@ -523,6 +518,12 @@
   </si>
   <si>
     <t>If [Attachments](attachments.html) is supported, the Data Source Client **SHALL**  support the `$submit-attachment` operation.</t>
+  </si>
+  <si>
+    <t>This CapabilityStatement describes the expected capabilities of a Da Vinci CDex Data Source (often an EHR) in *Client* mode during a clinical data exchange with a Data Consumer. This includes the following interactions:
+1. POSTing the `$submit-attachment` operation to exchange clinical data using a FHIR based Attachments transaction.
+1. Query for Authorization information represented by a CommunicationRequest or ServiceRequest.
+1. Posting a subscription notification to a Data Consumer endpoint updating the status of a Task.</t>
   </si>
 </sst>
 </file>
@@ -2307,8 +2308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2354,7 +2355,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2370,7 +2371,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2451,16 +2452,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -2468,16 +2469,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>134</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2563,19 +2564,19 @@
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="C2" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2796,13 +2797,13 @@
     </row>
     <row r="5" spans="1:25" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2825,7 +2826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -2857,19 +2858,19 @@
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2909,10 +2910,10 @@
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>102</v>

</xml_diff>